<commit_message>
Finish notebook Handling Missing values
</commit_message>
<xml_diff>
--- a/data/names_and_ages.xlsx
+++ b/data/names_and_ages.xlsx
@@ -5,22 +5,58 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\PySpark_projects\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\PySpark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04636459-64C9-4B7E-8C78-1C51C9D040B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD207B-F684-4222-A46D-201461CB195E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -176,13 +212,55 @@
   </si>
   <si>
     <t>Experience</t>
+  </si>
+  <si>
+    <t>ID job</t>
+  </si>
+  <si>
+    <t>Current Position</t>
+  </si>
+  <si>
+    <t>ID Position</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Sales Associate</t>
+  </si>
+  <si>
+    <t>Marketing Manager</t>
+  </si>
+  <si>
+    <t>Financial Analyst</t>
+  </si>
+  <si>
+    <t>Human Resources Specialist</t>
+  </si>
+  <si>
+    <t>Customer Service Representative</t>
+  </si>
+  <si>
+    <t>Graphic Designer</t>
+  </si>
+  <si>
+    <t>Operations Manager</t>
+  </si>
+  <si>
+    <t>Salary_USD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +272,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,11 +318,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,8 +646,17 @@
       <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -572,8 +666,20 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(1500,40000)</f>
+        <v>2911</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>9</v>
+      </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E2)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -583,8 +689,20 @@
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D50" ca="1" si="0">RANDBETWEEN(1500,20000)</f>
+        <v>3443</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E50" ca="1" si="1">RANDBETWEEN(1,10)</f>
+        <v>2</v>
+      </c>
+      <c r="F3" t="str" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E3)</f>
+        <v>Data Scientist</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -594,8 +712,20 @@
       <c r="C4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7034</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E4)</f>
+        <v>Marketing Manager</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -605,8 +735,20 @@
       <c r="C5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9118</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F5" t="str" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E5)</f>
+        <v>Financial Analyst</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -616,8 +758,20 @@
       <c r="C6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>12455</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="str" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E6)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -627,8 +781,20 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>8372</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" t="str" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E7)</f>
+        <v>Software Engineer</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -638,8 +804,20 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2443</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F8" t="str" cm="1">
+        <f t="array" aca="1" ref="F8" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E8)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -649,8 +827,20 @@
       <c r="C9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7750</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F9" t="str" cm="1">
+        <f t="array" aca="1" ref="F9" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E9)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -660,8 +850,20 @@
       <c r="C10">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3635</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F10" t="str" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E10)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -671,8 +873,20 @@
       <c r="C11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
+        <v>15356</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F11" t="str" cm="1">
+        <f t="array" aca="1" ref="F11" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E11)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -682,8 +896,20 @@
       <c r="C12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1940</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F12" t="str" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E12)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -693,8 +919,20 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" ca="1" si="0"/>
+        <v>4865</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F13" t="str" cm="1">
+        <f t="array" aca="1" ref="F13" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E13)</f>
+        <v>Customer Service Representative</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -704,8 +942,20 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1883</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F14" t="str" cm="1">
+        <f t="array" aca="1" ref="F14" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E14)</f>
+        <v>Customer Service Representative</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -715,8 +965,20 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" ca="1" si="0"/>
+        <v>7096</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F15" t="str" cm="1">
+        <f t="array" aca="1" ref="F15" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E15)</f>
+        <v>Project Manager</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -726,8 +988,20 @@
       <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6736</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F16" t="str" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E16)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -737,8 +1011,20 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2120</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F17" t="str" cm="1">
+        <f t="array" aca="1" ref="F17" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E17)</f>
+        <v>Project Manager</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -748,8 +1034,20 @@
       <c r="C18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" ca="1" si="0"/>
+        <v>16975</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F18" t="str" cm="1">
+        <f t="array" aca="1" ref="F18" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E18)</f>
+        <v>Project Manager</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -759,8 +1057,20 @@
       <c r="C19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2238</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F19" t="str" cm="1">
+        <f t="array" aca="1" ref="F19" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E19)</f>
+        <v>Software Engineer</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -770,8 +1080,20 @@
       <c r="C20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" ca="1" si="0"/>
+        <v>6936</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F20" t="str" cm="1">
+        <f t="array" aca="1" ref="F20" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E20)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -781,8 +1103,20 @@
       <c r="C21">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" ca="1" si="0"/>
+        <v>7815</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F21" t="str" cm="1">
+        <f t="array" aca="1" ref="F21" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E21)</f>
+        <v>Data Scientist</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -792,8 +1126,20 @@
       <c r="C22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" ca="1" si="0"/>
+        <v>3026</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F22" t="str" cm="1">
+        <f t="array" aca="1" ref="F22" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E22)</f>
+        <v>Project Manager</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -803,8 +1149,20 @@
       <c r="C23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" ca="1" si="0"/>
+        <v>8174</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F23" t="str" cm="1">
+        <f t="array" aca="1" ref="F23" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E23)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -814,8 +1172,20 @@
       <c r="C24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" ca="1" si="0"/>
+        <v>5596</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F24" t="str" cm="1">
+        <f t="array" aca="1" ref="F24" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E24)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -825,8 +1195,20 @@
       <c r="C25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" ca="1" si="0"/>
+        <v>19054</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F25" t="str" cm="1">
+        <f t="array" aca="1" ref="F25" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E25)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -836,8 +1218,20 @@
       <c r="C26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" ca="1" si="0"/>
+        <v>12362</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F26" t="str" cm="1">
+        <f t="array" aca="1" ref="F26" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E26)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -847,8 +1241,20 @@
       <c r="C27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" ca="1" si="0"/>
+        <v>6746</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F27" t="str" cm="1">
+        <f t="array" aca="1" ref="F27" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E27)</f>
+        <v>Financial Analyst</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -858,8 +1264,20 @@
       <c r="C28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" ca="1" si="0"/>
+        <v>5179</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F28" t="str" cm="1">
+        <f t="array" aca="1" ref="F28" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E28)</f>
+        <v>Customer Service Representative</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -869,8 +1287,20 @@
       <c r="C29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" ca="1" si="0"/>
+        <v>6242</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F29" t="str" cm="1">
+        <f t="array" aca="1" ref="F29" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E29)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -880,8 +1310,20 @@
       <c r="C30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" ca="1" si="0"/>
+        <v>8412</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F30" t="str" cm="1">
+        <f t="array" aca="1" ref="F30" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E30)</f>
+        <v>Financial Analyst</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -891,8 +1333,20 @@
       <c r="C31">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" ca="1" si="0"/>
+        <v>11092</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F31" t="str" cm="1">
+        <f t="array" aca="1" ref="F31" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E31)</f>
+        <v>Data Scientist</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -902,8 +1356,20 @@
       <c r="C32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" ca="1" si="0"/>
+        <v>6996</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F32" t="str" cm="1">
+        <f t="array" aca="1" ref="F32" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E32)</f>
+        <v>Software Engineer</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -913,8 +1379,20 @@
       <c r="C33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" ca="1" si="0"/>
+        <v>11485</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F33" t="str" cm="1">
+        <f t="array" aca="1" ref="F33" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E33)</f>
+        <v>Marketing Manager</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -924,8 +1402,20 @@
       <c r="C34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" ca="1" si="0"/>
+        <v>14278</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F34" t="str" cm="1">
+        <f t="array" aca="1" ref="F34" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E34)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -935,8 +1425,20 @@
       <c r="C35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" ca="1" si="0"/>
+        <v>12213</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F35" t="str" cm="1">
+        <f t="array" aca="1" ref="F35" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E35)</f>
+        <v>Data Scientist</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -946,8 +1448,20 @@
       <c r="C36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" ca="1" si="0"/>
+        <v>1965</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F36" t="str" cm="1">
+        <f t="array" aca="1" ref="F36" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E36)</f>
+        <v>Sales Associate</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -957,8 +1471,20 @@
       <c r="C37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" ca="1" si="0"/>
+        <v>10900</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F37" t="str" cm="1">
+        <f t="array" aca="1" ref="F37" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E37)</f>
+        <v>Sales Associate</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -968,8 +1494,20 @@
       <c r="C38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" ca="1" si="0"/>
+        <v>1602</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F38" t="str" cm="1">
+        <f t="array" aca="1" ref="F38" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E38)</f>
+        <v>Software Engineer</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -979,8 +1517,20 @@
       <c r="C39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" ca="1" si="0"/>
+        <v>14483</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F39" t="str" cm="1">
+        <f t="array" aca="1" ref="F39" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E39)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -990,8 +1540,20 @@
       <c r="C40">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" ca="1" si="0"/>
+        <v>17440</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F40" t="str" cm="1">
+        <f t="array" aca="1" ref="F40" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E40)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1001,8 +1563,20 @@
       <c r="C41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" ca="1" si="0"/>
+        <v>4811</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F41" t="str" cm="1">
+        <f t="array" aca="1" ref="F41" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E41)</f>
+        <v>Marketing Manager</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1012,8 +1586,20 @@
       <c r="C42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" ca="1" si="0"/>
+        <v>5530</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F42" t="str" cm="1">
+        <f t="array" aca="1" ref="F42" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E42)</f>
+        <v>Software Engineer</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1023,8 +1609,20 @@
       <c r="C43">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" ca="1" si="0"/>
+        <v>13287</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F43" t="str" cm="1">
+        <f t="array" aca="1" ref="F43" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E43)</f>
+        <v>Sales Associate</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1034,8 +1632,20 @@
       <c r="C44">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" ca="1" si="0"/>
+        <v>11555</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F44" t="str" cm="1">
+        <f t="array" aca="1" ref="F44" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E44)</f>
+        <v>Human Resources Specialist</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1045,8 +1655,20 @@
       <c r="C45">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" ca="1" si="0"/>
+        <v>8562</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F45" t="str" cm="1">
+        <f t="array" aca="1" ref="F45" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E45)</f>
+        <v>Marketing Manager</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1056,8 +1678,20 @@
       <c r="C46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" ca="1" si="0"/>
+        <v>13628</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F46" t="str" cm="1">
+        <f t="array" aca="1" ref="F46" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E46)</f>
+        <v>Graphic Designer</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1067,8 +1701,20 @@
       <c r="C47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" ca="1" si="0"/>
+        <v>10230</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F47" t="str" cm="1">
+        <f t="array" aca="1" ref="F47" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E47)</f>
+        <v>Operations Manager</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1078,8 +1724,20 @@
       <c r="C48">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" ca="1" si="0"/>
+        <v>8001</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F48" t="str" cm="1">
+        <f t="array" aca="1" ref="F48" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E48)</f>
+        <v>Financial Analyst</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1089,8 +1747,20 @@
       <c r="C49">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" ca="1" si="0"/>
+        <v>16315</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F49" t="str" cm="1">
+        <f t="array" aca="1" ref="F49" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E49)</f>
+        <v>Project Manager</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1099,6 +1769,121 @@
       </c>
       <c r="C50">
         <v>16</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="0"/>
+        <v>6166</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F50" t="str" cm="1">
+        <f t="array" aca="1" ref="F50" ca="1">INDEX(Hoja1!$B$2:$B$11,Sheet1!E50)</f>
+        <v>Financial Analyst</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C0D5C4-C7D7-4318-90B4-0781A420FA7C}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>